<commit_message>
update material add column sell
</commit_message>
<xml_diff>
--- a/src/main/java/com/coffee/ImportExcel/excel_ template/Materials.xlsx
+++ b/src/main/java/com/coffee/ImportExcel/excel_ template/Materials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\cafe_application\src\main\java\com\coffee\ImportExcel\excel_ template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72EE03D-9BEC-4E0B-A783-B3E5D768A3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7C03BD-06D0-4F5D-8422-3F696FF116C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3984" yWindow="2328" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Tên nguyên liệu</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>Bán trưc tiếp</t>
   </si>
 </sst>
 </file>
@@ -381,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -392,9 +395,10 @@
     <col min="1" max="1" width="14.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +414,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -427,8 +434,11 @@
       <c r="E2">
         <v>40000</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -444,8 +454,11 @@
       <c r="E3">
         <v>200</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -460,6 +473,9 @@
       </c>
       <c r="E4">
         <v>1000</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>